<commit_message>
pdf ajouté et messages formulaires en fr
</commit_message>
<xml_diff>
--- a/Audit-SEO-La chouette agence.xlsx
+++ b/Audit-SEO-La chouette agence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Bureau\Openclassrooms\Projet 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\Bureau\Openclassrooms\Projet 4\AlexandreAudigie_4_16_02_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Print_Area" localSheetId="0">Feuil1!$A$1:$H$13</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>Catégorie</t>
   </si>
@@ -188,9 +191,6 @@
     <t>Il faut supprimer tout code inutilisé ou qui se répéte</t>
   </si>
   <si>
-    <t>J'ai utilisé unCSS pour détecter le code inutilisé et le supprimer</t>
-  </si>
-  <si>
     <t>https://fr.docs.wp-rocket.me/article/1577-supprimer-les-ressources-css-inutilisees</t>
   </si>
   <si>
@@ -201,24 +201,23 @@
   </si>
   <si>
     <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941406-rendez-les-interactions-sur-le-site-accessibles</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>J'ai utilisé unCSS pour détecter le code inutilisé et le supprimer, j'ai également minifier les fichiers css et javascript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -244,6 +243,31 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -259,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,26 +292,178 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -504,291 +680,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="26" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" customWidth="1"/>
+    <col min="7" max="7" width="55.21875" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" customWidth="1"/>
+    <col min="9" max="27" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:27" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="10"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:27" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:27" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:27" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:27" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="10"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
+    <row r="8" spans="1:27" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="10"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
+    <row r="9" spans="1:27" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:27" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="10"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
-      </c>
+    <row r="11" spans="1:27" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="10"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:27" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="C12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>39</v>
-      </c>
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>49</v>
-      </c>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>54</v>
-      </c>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>44</v>
-      </c>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="4"/>
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1757,20 +1978,22 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F11" r:id="rId7" location=":~:text=En%20effet%2C%20le%20W3C%20a,est%20100%25%20conforme%20au%20standard."/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F5" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G7" r:id="rId4"/>
+    <hyperlink ref="G9" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G12" r:id="rId7" location=":~:text=En%20effet%2C%20le%20W3C%20a,est%20100%25%20conforme%20au%20standard."/>
+    <hyperlink ref="G10" r:id="rId8"/>
+    <hyperlink ref="G11" r:id="rId9"/>
+    <hyperlink ref="G6" r:id="rId10"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.19685039370078741" bottom="0.15748031496062992" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>